<commit_message>
Add GPS section to nav hardware comparison
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/avionics/nav-hardware-compare.xlsx
+++ b/docs/avionics/nav-hardware-compare.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARC\Research\docs\avionics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487B9F30-50D6-4005-A87D-6DEEDBD2E6A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C23B93E-5953-45A8-A80E-FA50CB1F8B27}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{45348F4D-BE45-4D91-992A-D063F65F5299}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{45348F4D-BE45-4D91-992A-D063F65F5299}"/>
   </bookViews>
   <sheets>
     <sheet name="IMU" sheetId="1" r:id="rId1"/>
+    <sheet name="GPS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="130">
   <si>
     <t>Metric</t>
   </si>
@@ -244,6 +245,183 @@
   </si>
   <si>
     <t>POST, BIST</t>
+  </si>
+  <si>
+    <t>NEO-M8Q-01A</t>
+  </si>
+  <si>
+    <t>Integrated antenna</t>
+  </si>
+  <si>
+    <t>Antenna interfaces</t>
+  </si>
+  <si>
+    <t># concurrent GNSS</t>
+  </si>
+  <si>
+    <t>Multi-GNSS</t>
+  </si>
+  <si>
+    <t>GNSS type</t>
+  </si>
+  <si>
+    <t>Oscillator</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>MAX-8C</t>
+  </si>
+  <si>
+    <t>MAX-8Q</t>
+  </si>
+  <si>
+    <t>LEA-M8S</t>
+  </si>
+  <si>
+    <t>ublox</t>
+  </si>
+  <si>
+    <t>12.2 mm</t>
+  </si>
+  <si>
+    <t>16 mm</t>
+  </si>
+  <si>
+    <t>2.4 mm</t>
+  </si>
+  <si>
+    <t>-40 - 105 degC</t>
+  </si>
+  <si>
+    <t>2.70-3.6 V</t>
+  </si>
+  <si>
+    <t>BeiDou, Galileo, GLONASS, GPS/QZSS</t>
+  </si>
+  <si>
+    <t>TCXO</t>
+  </si>
+  <si>
+    <t># channels</t>
+  </si>
+  <si>
+    <t>Limit: altitude</t>
+  </si>
+  <si>
+    <t>Limit: velocity</t>
+  </si>
+  <si>
+    <t>500 m/s</t>
+  </si>
+  <si>
+    <t>Velocity accuracy</t>
+  </si>
+  <si>
+    <t>Heading accuracy</t>
+  </si>
+  <si>
+    <t>TTFF cold-start</t>
+  </si>
+  <si>
+    <t>TTFF hot-start</t>
+  </si>
+  <si>
+    <t>TTFF aided-start</t>
+  </si>
+  <si>
+    <t>0.3 deg</t>
+  </si>
+  <si>
+    <t>0.05 m/s</t>
+  </si>
+  <si>
+    <t>26 sec</t>
+  </si>
+  <si>
+    <t>1 sec</t>
+  </si>
+  <si>
+    <t>2 sec</t>
+  </si>
+  <si>
+    <t>Sensitivity track&amp;nav</t>
+  </si>
+  <si>
+    <t>Sensitivity reacquisition</t>
+  </si>
+  <si>
+    <t>Sensitivity cold-start</t>
+  </si>
+  <si>
+    <t>Sensitivity hot-start</t>
+  </si>
+  <si>
+    <t>-167 dBm</t>
+  </si>
+  <si>
+    <t>-160 dBm</t>
+  </si>
+  <si>
+    <t>-148 dBm</t>
+  </si>
+  <si>
+    <t>-157 dBm</t>
+  </si>
+  <si>
+    <t>UART, USB, SPI, DDC</t>
+  </si>
+  <si>
+    <t>9.7 mm</t>
+  </si>
+  <si>
+    <t>10.1 mm</t>
+  </si>
+  <si>
+    <t>2.5 mm</t>
+  </si>
+  <si>
+    <t>1.65-3.6 V</t>
+  </si>
+  <si>
+    <t>-40 - 85 degC</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>GLONASS, GPS/QZSS</t>
+  </si>
+  <si>
+    <t>50000 m</t>
+  </si>
+  <si>
+    <t>5000 m</t>
+  </si>
+  <si>
+    <t>29 sec</t>
+  </si>
+  <si>
+    <t>30 sec</t>
+  </si>
+  <si>
+    <t>3 sec</t>
+  </si>
+  <si>
+    <t>-164 dBm</t>
+  </si>
+  <si>
+    <t>-159 dBm</t>
+  </si>
+  <si>
+    <t>-147 dBm</t>
+  </si>
+  <si>
+    <t>-156 dBm</t>
+  </si>
+  <si>
+    <t>-166 dBm</t>
   </si>
 </sst>
 </file>
@@ -317,6 +495,20 @@
     <tableColumn id="9" xr3:uid="{0DF6D068-1387-4521-A7C2-D24D2DA91D34}" name="BNO055" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{04702736-6AFD-4512-AF89-1C2A09D9DCD3}" name="Table2" displayName="Table2" ref="A1:E32" totalsRowShown="0">
+  <autoFilter ref="A1:E32" xr:uid="{8040AE00-58DA-439D-815B-777F5227B716}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2D51013C-8C20-4AC9-B5B5-A03ABA0CC7AF}" name="Metric"/>
+    <tableColumn id="2" xr3:uid="{C27B7664-1E3C-4879-8C79-28B1E9A1F763}" name="NEO-M8Q-01A"/>
+    <tableColumn id="3" xr3:uid="{C332229B-9F36-4DEE-ACA1-4AEDF3B2F49C}" name="MAX-8C"/>
+    <tableColumn id="4" xr3:uid="{339F9C17-B996-4957-BC88-182AEECCEF62}" name="MAX-8Q"/>
+    <tableColumn id="5" xr3:uid="{CADC7510-26D5-45F5-B3A9-5E2F2D53D856}" name="LEA-M8S"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -622,8 +814,8 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
@@ -1111,4 +1303,416 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50BCB51-82B5-48D2-BD5C-171740C85E68}">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="21.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.05078125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21">
+        <v>72</v>
+      </c>
+      <c r="C21">
+        <v>72</v>
+      </c>
+      <c r="D21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>